<commit_message>
code citations double checked
</commit_message>
<xml_diff>
--- a/Test_Journey_get_offroute_data_df_route.xlsx
+++ b/Test_Journey_get_offroute_data_df_route.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,41 +424,41 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G2" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H2" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I2" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J2" t="n">
-        <v>51.28588</v>
+        <v>51.22234</v>
       </c>
       <c r="K2" t="n">
-        <v>-2.48243</v>
+        <v>-2.31109</v>
       </c>
     </row>
     <row r="3">
@@ -467,41 +467,41 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G3" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H3" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I3" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J3" t="n">
-        <v>51.28069</v>
+        <v>51.22237</v>
       </c>
       <c r="K3" t="n">
-        <v>-2.48258</v>
+        <v>-2.3107</v>
       </c>
     </row>
     <row r="4">
@@ -510,41 +510,41 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G4" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H4" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I4" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J4" t="n">
-        <v>51.27766</v>
+        <v>51.22273</v>
       </c>
       <c r="K4" t="n">
-        <v>-2.47367</v>
+        <v>-2.31064</v>
       </c>
     </row>
     <row r="5">
@@ -553,41 +553,41 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G5" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H5" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I5" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J5" t="n">
-        <v>51.24146</v>
+        <v>51.22283</v>
       </c>
       <c r="K5" t="n">
-        <v>-2.50109</v>
+        <v>-2.31005</v>
       </c>
     </row>
     <row r="6">
@@ -596,41 +596,41 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G6" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H6" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I6" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J6" t="n">
-        <v>51.23749</v>
+        <v>51.22298</v>
       </c>
       <c r="K6" t="n">
-        <v>-2.49996</v>
+        <v>-2.30982</v>
       </c>
     </row>
     <row r="7">
@@ -639,41 +639,41 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G7" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H7" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I7" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J7" t="n">
-        <v>51.22464</v>
+        <v>51.22374</v>
       </c>
       <c r="K7" t="n">
-        <v>-2.52279</v>
+        <v>-2.30909</v>
       </c>
     </row>
     <row r="8">
@@ -682,41 +682,41 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G8" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H8" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I8" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J8" t="n">
-        <v>51.21931</v>
+        <v>51.22498</v>
       </c>
       <c r="K8" t="n">
-        <v>-2.52331</v>
+        <v>-2.30754</v>
       </c>
     </row>
     <row r="9">
@@ -725,41 +725,41 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G9" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H9" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I9" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J9" t="n">
-        <v>51.21723</v>
+        <v>51.22534</v>
       </c>
       <c r="K9" t="n">
-        <v>-2.53102</v>
+        <v>-2.30686</v>
       </c>
     </row>
     <row r="10">
@@ -768,41 +768,41 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G10" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H10" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I10" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J10" t="n">
-        <v>51.20703</v>
+        <v>51.22581</v>
       </c>
       <c r="K10" t="n">
-        <v>-2.53952</v>
+        <v>-2.3054</v>
       </c>
     </row>
     <row r="11">
@@ -811,41 +811,41 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G11" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H11" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I11" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J11" t="n">
-        <v>51.17033</v>
+        <v>51.22681</v>
       </c>
       <c r="K11" t="n">
-        <v>-2.53426</v>
+        <v>-2.30373</v>
       </c>
     </row>
     <row r="12">
@@ -854,41 +854,41 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G12" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H12" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I12" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J12" t="n">
-        <v>51.1622</v>
+        <v>51.22708</v>
       </c>
       <c r="K12" t="n">
-        <v>-2.52448</v>
+        <v>-2.30363</v>
       </c>
     </row>
     <row r="13">
@@ -897,41 +897,41 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G13" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H13" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I13" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J13" t="n">
-        <v>51.13935</v>
+        <v>51.22726</v>
       </c>
       <c r="K13" t="n">
-        <v>-2.5165</v>
+        <v>-2.30377</v>
       </c>
     </row>
     <row r="14">
@@ -940,41 +940,41 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G14" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H14" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I14" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J14" t="n">
-        <v>51.11793</v>
+        <v>51.22884</v>
       </c>
       <c r="K14" t="n">
-        <v>-2.51654</v>
+        <v>-2.3063</v>
       </c>
     </row>
     <row r="15">
@@ -983,41 +983,41 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G15" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H15" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I15" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J15" t="n">
-        <v>51.09809</v>
+        <v>51.22893</v>
       </c>
       <c r="K15" t="n">
-        <v>-2.5272</v>
+        <v>-2.30699</v>
       </c>
     </row>
     <row r="16">
@@ -1026,41 +1026,41 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G16" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H16" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I16" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J16" t="n">
-        <v>51.09568</v>
+        <v>51.22876</v>
       </c>
       <c r="K16" t="n">
-        <v>-2.51432</v>
+        <v>-2.30829</v>
       </c>
     </row>
     <row r="17">
@@ -1069,41 +1069,41 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G17" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H17" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I17" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J17" t="n">
-        <v>51.0883</v>
+        <v>51.22791</v>
       </c>
       <c r="K17" t="n">
-        <v>-2.50516</v>
+        <v>-2.31099</v>
       </c>
     </row>
     <row r="18">
@@ -1112,41 +1112,41 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G18" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H18" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I18" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J18" t="n">
-        <v>51.08085</v>
+        <v>51.22768</v>
       </c>
       <c r="K18" t="n">
-        <v>-2.50525</v>
+        <v>-2.31325</v>
       </c>
     </row>
     <row r="19">
@@ -1155,41 +1155,41 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G19" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H19" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I19" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J19" t="n">
-        <v>51.07437</v>
+        <v>51.22642</v>
       </c>
       <c r="K19" t="n">
-        <v>-2.48541</v>
+        <v>-2.31437</v>
       </c>
     </row>
     <row r="20">
@@ -1198,41 +1198,41 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G20" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H20" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I20" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J20" t="n">
-        <v>51.06502</v>
+        <v>51.22582</v>
       </c>
       <c r="K20" t="n">
-        <v>-2.48095</v>
+        <v>-2.31544</v>
       </c>
     </row>
     <row r="21">
@@ -1241,41 +1241,41 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G21" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H21" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I21" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J21" t="n">
-        <v>51.06064</v>
+        <v>51.22519</v>
       </c>
       <c r="K21" t="n">
-        <v>-2.45763</v>
+        <v>-2.31769</v>
       </c>
     </row>
     <row r="22">
@@ -1284,41 +1284,41 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G22" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H22" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I22" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J22" t="n">
-        <v>51.04719</v>
+        <v>51.22484</v>
       </c>
       <c r="K22" t="n">
-        <v>-2.4342</v>
+        <v>-2.32133</v>
       </c>
     </row>
     <row r="23">
@@ -1327,41 +1327,41 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G23" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H23" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I23" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J23" t="n">
-        <v>51.02151</v>
+        <v>51.22421</v>
       </c>
       <c r="K23" t="n">
-        <v>-2.43949</v>
+        <v>-2.32144</v>
       </c>
     </row>
     <row r="24">
@@ -1370,41 +1370,41 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G24" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H24" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I24" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J24" t="n">
-        <v>51.00158</v>
+        <v>51.22301</v>
       </c>
       <c r="K24" t="n">
-        <v>-2.41545</v>
+        <v>-2.32124</v>
       </c>
     </row>
     <row r="25">
@@ -1413,41 +1413,41 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G25" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H25" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I25" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J25" t="n">
-        <v>50.9973</v>
+        <v>51.22183</v>
       </c>
       <c r="K25" t="n">
-        <v>-2.41614</v>
+        <v>-2.32125</v>
       </c>
     </row>
     <row r="26">
@@ -1456,41 +1456,213 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BA3 2HW</t>
+          <t>BA11 5LB</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>BA8 0SJ</t>
+          <t>BA11 5AP</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>15 High Street, Midsomer Norton, Radstock, BA3 2HW, United Kingdom</t>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>19 Woodhayes, Henstridge, Templecombe, BA8 0SJ, United Kingdom</t>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>43.74630000000001</v>
+        <v>3.0501</v>
       </c>
       <c r="G26" t="n">
-        <v>43746.3</v>
+        <v>3050.1</v>
       </c>
       <c r="H26" t="n">
-        <v>60.85</v>
+        <v>8.711666666666668</v>
       </c>
       <c r="I26" t="n">
-        <v>3651</v>
+        <v>522.7</v>
       </c>
       <c r="J26" t="n">
-        <v>50.97474</v>
+        <v>51.22048</v>
       </c>
       <c r="K26" t="n">
-        <v>-2.39394</v>
+        <v>-2.32074</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>BA11 5LB</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>BA11 5AP</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>3.0501</v>
+      </c>
+      <c r="G27" t="n">
+        <v>3050.1</v>
+      </c>
+      <c r="H27" t="n">
+        <v>8.711666666666668</v>
+      </c>
+      <c r="I27" t="n">
+        <v>522.7</v>
+      </c>
+      <c r="J27" t="n">
+        <v>51.22034</v>
+      </c>
+      <c r="K27" t="n">
+        <v>-2.31956</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>BA11 5LB</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>BA11 5AP</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>3.0501</v>
+      </c>
+      <c r="G28" t="n">
+        <v>3050.1</v>
+      </c>
+      <c r="H28" t="n">
+        <v>8.711666666666668</v>
+      </c>
+      <c r="I28" t="n">
+        <v>522.7</v>
+      </c>
+      <c r="J28" t="n">
+        <v>51.21988</v>
+      </c>
+      <c r="K28" t="n">
+        <v>-2.31827</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>BA11 5LB</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>BA11 5AP</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>3.0501</v>
+      </c>
+      <c r="G29" t="n">
+        <v>3050.1</v>
+      </c>
+      <c r="H29" t="n">
+        <v>8.711666666666668</v>
+      </c>
+      <c r="I29" t="n">
+        <v>522.7</v>
+      </c>
+      <c r="J29" t="n">
+        <v>51.22045</v>
+      </c>
+      <c r="K29" t="n">
+        <v>-2.31728</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>BA11 5LB</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>BA11 5AP</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>81 Knights Maltings, Frome, Frome, BA11 5LB, United Kingdom</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>55 Tower View, Frome, Frome, BA11 5AP, United Kingdom</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>3.0501</v>
+      </c>
+      <c r="G30" t="n">
+        <v>3050.1</v>
+      </c>
+      <c r="H30" t="n">
+        <v>8.711666666666668</v>
+      </c>
+      <c r="I30" t="n">
+        <v>522.7</v>
+      </c>
+      <c r="J30" t="n">
+        <v>51.22032</v>
+      </c>
+      <c r="K30" t="n">
+        <v>-2.31717</v>
       </c>
     </row>
   </sheetData>

</xml_diff>